<commit_message>
Se actualizó el burndown
</commit_message>
<xml_diff>
--- a/proyecto/Burndown chart.xlsx
+++ b/proyecto/Burndown chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aburtoad\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C5FFA9-97B4-4BCA-ADCA-23A1FD143860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89798AB2-1B56-498B-BCF0-AEA70728FB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{0544001C-EE5B-4143-BFFE-3772AB433641}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0544001C-EE5B-4143-BFFE-3772AB433641}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>Historia de Usuario</t>
   </si>
@@ -299,6 +299,12 @@
   <si>
     <t>Hacer navbar responsivo</t>
   </si>
+  <si>
+    <t>Google analytics</t>
+  </si>
+  <si>
+    <t>Frontend pantalla de inicio</t>
+  </si>
 </sst>
 </file>
 
@@ -340,7 +346,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,6 +374,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -400,7 +418,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -423,7 +441,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -445,6 +462,29 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -498,7 +538,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$17</c:f>
+              <c:f>Sheet1!$B$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -523,174 +563,225 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$BE$17</c:f>
+              <c:f>Sheet1!$C$19:$BV$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>43</c:v>
+                <c:pt idx="6">
+                  <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="17">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="18">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="19">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>32</c:v>
-                </c:pt>
                 <c:pt idx="21">
-                  <c:v>32</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>32</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>32</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>31</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>31</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="28">
-                  <c:v>27</c:v>
-                </c:pt>
                 <c:pt idx="29">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="33">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="34">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="36">
-                  <c:v>23</c:v>
-                </c:pt>
                 <c:pt idx="37">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="41">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="42">
-                  <c:v>18</c:v>
-                </c:pt>
                 <c:pt idx="43">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -707,7 +798,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$18</c:f>
+              <c:f>Sheet1!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -730,174 +821,225 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$BE$18</c:f>
+              <c:f>Sheet1!$C$20:$BV$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="55"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>46</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45.352112676056336</c:v>
+                  <c:v>49.295774647887328</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44.704225352112672</c:v>
+                  <c:v>48.591549295774648</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44.056338028169016</c:v>
+                  <c:v>47.887323943661968</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43.408450704225352</c:v>
+                  <c:v>47.183098591549296</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42.760563380281688</c:v>
+                  <c:v>46.478873239436624</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42.112676056338032</c:v>
+                  <c:v>45.774647887323944</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41.464788732394368</c:v>
+                  <c:v>45.070422535211264</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.816901408450704</c:v>
+                  <c:v>44.366197183098592</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40.16901408450704</c:v>
+                  <c:v>43.661971830985919</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>39.521126760563376</c:v>
+                  <c:v>42.95774647887324</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>38.87323943661972</c:v>
+                  <c:v>42.25352112676056</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>38.225352112676056</c:v>
+                  <c:v>41.549295774647888</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>37.577464788732392</c:v>
+                  <c:v>40.845070422535215</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>36.929577464788736</c:v>
+                  <c:v>40.140845070422536</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>36.281690140845072</c:v>
+                  <c:v>39.436619718309856</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>35.633802816901408</c:v>
+                  <c:v>38.732394366197184</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>34.985915492957744</c:v>
+                  <c:v>38.028169014084511</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>34.338028169014081</c:v>
+                  <c:v>37.323943661971832</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>33.690140845070424</c:v>
+                  <c:v>36.619718309859152</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>33.04225352112676</c:v>
+                  <c:v>35.91549295774648</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>32.394366197183096</c:v>
+                  <c:v>35.211267605633807</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>31.746478873239436</c:v>
+                  <c:v>34.507042253521128</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>31.098591549295776</c:v>
+                  <c:v>33.802816901408448</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>30.450704225352112</c:v>
+                  <c:v>33.098591549295776</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>29.802816901408448</c:v>
+                  <c:v>32.394366197183103</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>29.154929577464788</c:v>
+                  <c:v>31.690140845070424</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>28.507042253521128</c:v>
+                  <c:v>30.985915492957748</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>27.859154929577464</c:v>
+                  <c:v>30.281690140845072</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>27.2112676056338</c:v>
+                  <c:v>29.577464788732396</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>26.56338028169014</c:v>
+                  <c:v>28.87323943661972</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>25.91549295774648</c:v>
+                  <c:v>28.169014084507044</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>25.267605633802816</c:v>
+                  <c:v>27.464788732394368</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>24.619718309859152</c:v>
+                  <c:v>26.760563380281692</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>23.971830985915492</c:v>
+                  <c:v>26.056338028169016</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>23.323943661971832</c:v>
+                  <c:v>25.35211267605634</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>22.676056338028168</c:v>
+                  <c:v>24.647887323943664</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>22.028169014084504</c:v>
+                  <c:v>23.943661971830988</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>21.380281690140844</c:v>
+                  <c:v>23.239436619718312</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>20.732394366197184</c:v>
+                  <c:v>22.535211267605636</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>20.08450704225352</c:v>
+                  <c:v>21.83098591549296</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>19.436619718309856</c:v>
+                  <c:v>21.126760563380284</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>18.788732394366196</c:v>
+                  <c:v>20.422535211267608</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>18.140845070422536</c:v>
+                  <c:v>19.718309859154932</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>17.492957746478872</c:v>
+                  <c:v>19.014084507042256</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>16.845070422535208</c:v>
+                  <c:v>18.30985915492958</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>16.197183098591548</c:v>
+                  <c:v>17.605633802816904</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>15.549295774647888</c:v>
+                  <c:v>16.901408450704224</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>14.901408450704224</c:v>
+                  <c:v>16.197183098591552</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>14.25352112676056</c:v>
+                  <c:v>15.492957746478879</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>13.605633802816897</c:v>
+                  <c:v>14.7887323943662</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>12.95774647887324</c:v>
+                  <c:v>14.08450704225352</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>12.309859154929576</c:v>
+                  <c:v>13.380281690140848</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>11.661971830985912</c:v>
+                  <c:v>12.676056338028175</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>11.014084507042256</c:v>
+                  <c:v>11.971830985915496</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>11.267605633802816</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>10.563380281690144</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>9.8591549295774712</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>9.1549295774647916</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>8.4507042253521121</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>7.7464788732394396</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>7.0422535211267672</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.3380281690140876</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5.6338028169014081</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4.9295774647887356</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4.2253521126760631</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.5211267605633836</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.816901408450704</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.1126760563380316</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.4084507042253591</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.70422535211267956</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1682,13 +1824,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>819346</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>168880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>555625</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>2096</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2014,10 +2156,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF382278-246E-4313-A951-9F92E3EB05C3}">
-  <dimension ref="A2:BV1002"/>
+  <dimension ref="A2:BV1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M75" sqref="M75"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="31" zoomScaleNormal="27" workbookViewId="0">
+      <selection activeCell="BD10" sqref="BD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2061,7 +2203,7 @@
     </row>
     <row r="3" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -2283,7 +2425,7 @@
     </row>
     <row r="4" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="17"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
@@ -2501,443 +2643,441 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:74" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5" spans="1:74" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="19">
         <v>3</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8">
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19">
         <v>1</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8">
+      <c r="G5" s="19"/>
+      <c r="H5" s="19">
         <v>1</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8">
+      <c r="I5" s="19"/>
+      <c r="J5" s="19">
         <v>1</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="9"/>
-      <c r="AE5" s="9"/>
-      <c r="AF5" s="9"/>
-      <c r="AG5" s="9"/>
-      <c r="AH5" s="9"/>
-      <c r="AI5" s="9"/>
-      <c r="AJ5" s="9"/>
-      <c r="AK5" s="9"/>
-      <c r="AL5" s="9"/>
-      <c r="AM5" s="9"/>
-      <c r="AN5" s="9"/>
-      <c r="AO5" s="9"/>
-      <c r="AP5" s="9"/>
-      <c r="AQ5" s="9"/>
-      <c r="AR5" s="9"/>
-      <c r="AS5" s="9"/>
-      <c r="AT5" s="9"/>
-      <c r="AU5" s="9"/>
-      <c r="AV5" s="9"/>
-      <c r="AW5" s="9"/>
-      <c r="AX5" s="9"/>
-      <c r="AY5" s="9"/>
-      <c r="AZ5" s="9"/>
-      <c r="BA5" s="9"/>
-      <c r="BB5" s="9"/>
-      <c r="BC5" s="9"/>
-      <c r="BD5" s="9"/>
-      <c r="BE5" s="9"/>
-      <c r="BF5" s="9"/>
-      <c r="BG5" s="9"/>
-      <c r="BH5" s="9"/>
-      <c r="BI5" s="9"/>
-      <c r="BJ5" s="9"/>
-      <c r="BK5" s="9"/>
-      <c r="BL5" s="9"/>
-      <c r="BM5" s="9"/>
-      <c r="BN5" s="9"/>
-      <c r="BO5" s="9"/>
-      <c r="BP5" s="9"/>
-      <c r="BQ5" s="9"/>
-      <c r="BR5" s="9"/>
-      <c r="BS5" s="9"/>
-      <c r="BT5" s="9"/>
-      <c r="BU5" s="9"/>
-      <c r="BV5" s="9"/>
-    </row>
-    <row r="6" spans="1:74" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="20"/>
+      <c r="AD5" s="20"/>
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="20"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="20"/>
+      <c r="AI5" s="20"/>
+      <c r="AJ5" s="20"/>
+      <c r="AK5" s="20"/>
+      <c r="AL5" s="20"/>
+      <c r="AM5" s="20"/>
+      <c r="AN5" s="20"/>
+      <c r="AO5" s="20"/>
+      <c r="AP5" s="20"/>
+      <c r="AQ5" s="20"/>
+      <c r="AR5" s="20"/>
+      <c r="AS5" s="20"/>
+      <c r="AT5" s="20"/>
+      <c r="AU5" s="20"/>
+      <c r="AV5" s="20"/>
+      <c r="AW5" s="20"/>
+      <c r="AX5" s="20"/>
+      <c r="AY5" s="20"/>
+      <c r="AZ5" s="20"/>
+      <c r="BA5" s="20"/>
+      <c r="BB5" s="20"/>
+      <c r="BC5" s="20"/>
+      <c r="BD5" s="20"/>
+      <c r="BE5" s="20"/>
+      <c r="BF5" s="20"/>
+      <c r="BG5" s="20"/>
+      <c r="BH5" s="20"/>
+      <c r="BI5" s="20"/>
+      <c r="BJ5" s="20"/>
+      <c r="BK5" s="20"/>
+      <c r="BL5" s="20"/>
+      <c r="BM5" s="20"/>
+      <c r="BN5" s="20"/>
+      <c r="BO5" s="20"/>
+      <c r="BP5" s="20"/>
+      <c r="BQ5" s="20"/>
+      <c r="BR5" s="20"/>
+      <c r="BS5" s="20"/>
+      <c r="BT5" s="20"/>
+      <c r="BU5" s="20"/>
+      <c r="BV5" s="20"/>
+    </row>
+    <row r="6" spans="1:74" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
         <v>2</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="19">
         <v>3</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8">
+      <c r="D6" s="19"/>
+      <c r="E6" s="19">
         <v>1</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8">
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19">
         <v>1</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="19">
         <v>1</v>
       </c>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="9"/>
-      <c r="AC6" s="9"/>
-      <c r="AD6" s="9"/>
-      <c r="AE6" s="9"/>
-      <c r="AF6" s="9"/>
-      <c r="AG6" s="9"/>
-      <c r="AH6" s="9"/>
-      <c r="AI6" s="9"/>
-      <c r="AJ6" s="9"/>
-      <c r="AK6" s="9"/>
-      <c r="AL6" s="9"/>
-      <c r="AM6" s="9"/>
-      <c r="AN6" s="9"/>
-      <c r="AO6" s="9"/>
-      <c r="AP6" s="9"/>
-      <c r="AQ6" s="9"/>
-      <c r="AR6" s="9"/>
-      <c r="AS6" s="9"/>
-      <c r="AT6" s="9"/>
-      <c r="AU6" s="9"/>
-      <c r="AV6" s="9"/>
-      <c r="AW6" s="9"/>
-      <c r="AX6" s="9"/>
-      <c r="AY6" s="9"/>
-      <c r="AZ6" s="9"/>
-      <c r="BA6" s="9"/>
-      <c r="BB6" s="9"/>
-      <c r="BC6" s="9"/>
-      <c r="BD6" s="9"/>
-      <c r="BE6" s="9"/>
-      <c r="BF6" s="9"/>
-      <c r="BG6" s="9"/>
-      <c r="BH6" s="9"/>
-      <c r="BI6" s="9"/>
-      <c r="BJ6" s="9"/>
-      <c r="BK6" s="9"/>
-      <c r="BL6" s="9"/>
-      <c r="BM6" s="9"/>
-      <c r="BN6" s="9"/>
-      <c r="BO6" s="9"/>
-      <c r="BP6" s="9"/>
-      <c r="BQ6" s="9"/>
-      <c r="BR6" s="9"/>
-      <c r="BS6" s="9"/>
-      <c r="BT6" s="9"/>
-      <c r="BU6" s="9"/>
-      <c r="BV6" s="9"/>
-    </row>
-    <row r="7" spans="1:74" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="20"/>
+      <c r="AD6" s="20"/>
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="20"/>
+      <c r="AG6" s="20"/>
+      <c r="AH6" s="20"/>
+      <c r="AI6" s="20"/>
+      <c r="AJ6" s="20"/>
+      <c r="AK6" s="20"/>
+      <c r="AL6" s="20"/>
+      <c r="AM6" s="20"/>
+      <c r="AN6" s="20"/>
+      <c r="AO6" s="20"/>
+      <c r="AP6" s="20"/>
+      <c r="AQ6" s="20"/>
+      <c r="AR6" s="20"/>
+      <c r="AS6" s="20"/>
+      <c r="AT6" s="20"/>
+      <c r="AU6" s="20"/>
+      <c r="AV6" s="20"/>
+      <c r="AW6" s="20"/>
+      <c r="AX6" s="20"/>
+      <c r="AY6" s="20"/>
+      <c r="AZ6" s="20"/>
+      <c r="BA6" s="20"/>
+      <c r="BB6" s="20"/>
+      <c r="BC6" s="20"/>
+      <c r="BD6" s="20"/>
+      <c r="BE6" s="20"/>
+      <c r="BF6" s="20"/>
+      <c r="BG6" s="20"/>
+      <c r="BH6" s="20"/>
+      <c r="BI6" s="20"/>
+      <c r="BJ6" s="20"/>
+      <c r="BK6" s="20"/>
+      <c r="BL6" s="20"/>
+      <c r="BM6" s="20"/>
+      <c r="BN6" s="20"/>
+      <c r="BO6" s="20"/>
+      <c r="BP6" s="20"/>
+      <c r="BQ6" s="20"/>
+      <c r="BR6" s="20"/>
+      <c r="BS6" s="20"/>
+      <c r="BT6" s="20"/>
+      <c r="BU6" s="20"/>
+      <c r="BV6" s="20"/>
+    </row>
+    <row r="7" spans="1:74" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="19">
         <v>3</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8">
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19">
         <v>1</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="19">
         <v>1</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8">
+      <c r="H7" s="22"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19">
         <v>1</v>
       </c>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="8"/>
-      <c r="AA7" s="9"/>
-      <c r="AB7" s="9"/>
-      <c r="AC7" s="9"/>
-      <c r="AD7" s="9"/>
-      <c r="AE7" s="9"/>
-      <c r="AF7" s="9"/>
-      <c r="AG7" s="9"/>
-      <c r="AH7" s="9"/>
-      <c r="AI7" s="9"/>
-      <c r="AJ7" s="9"/>
-      <c r="AK7" s="9"/>
-      <c r="AL7" s="9"/>
-      <c r="AM7" s="9"/>
-      <c r="AN7" s="9"/>
-      <c r="AO7" s="9"/>
-      <c r="AP7" s="9"/>
-      <c r="AQ7" s="9"/>
-      <c r="AR7" s="9"/>
-      <c r="AS7" s="9"/>
-      <c r="AT7" s="9"/>
-      <c r="AU7" s="9"/>
-      <c r="AV7" s="9"/>
-      <c r="AW7" s="9"/>
-      <c r="AX7" s="9"/>
-      <c r="AY7" s="9"/>
-      <c r="AZ7" s="9"/>
-      <c r="BA7" s="9"/>
-      <c r="BB7" s="9"/>
-      <c r="BC7" s="9"/>
-      <c r="BD7" s="9"/>
-      <c r="BE7" s="9"/>
-      <c r="BF7" s="9"/>
-      <c r="BG7" s="9"/>
-      <c r="BH7" s="9"/>
-      <c r="BI7" s="9"/>
-      <c r="BJ7" s="9"/>
-      <c r="BK7" s="9"/>
-      <c r="BL7" s="9"/>
-      <c r="BM7" s="9"/>
-      <c r="BN7" s="9"/>
-      <c r="BO7" s="9"/>
-      <c r="BP7" s="9"/>
-      <c r="BQ7" s="9"/>
-      <c r="BR7" s="9"/>
-      <c r="BS7" s="9"/>
-      <c r="BT7" s="9"/>
-      <c r="BU7" s="9"/>
-      <c r="BV7" s="9"/>
-    </row>
-    <row r="8" spans="1:74" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="20"/>
+      <c r="AD7" s="20"/>
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="20"/>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="20"/>
+      <c r="AI7" s="20"/>
+      <c r="AJ7" s="20"/>
+      <c r="AK7" s="20"/>
+      <c r="AL7" s="20"/>
+      <c r="AM7" s="20"/>
+      <c r="AN7" s="20"/>
+      <c r="AO7" s="20"/>
+      <c r="AP7" s="20"/>
+      <c r="AQ7" s="20"/>
+      <c r="AR7" s="20"/>
+      <c r="AS7" s="20"/>
+      <c r="AT7" s="20"/>
+      <c r="AU7" s="20"/>
+      <c r="AV7" s="20"/>
+      <c r="AW7" s="20"/>
+      <c r="AX7" s="20"/>
+      <c r="AY7" s="20"/>
+      <c r="AZ7" s="20"/>
+      <c r="BA7" s="20"/>
+      <c r="BB7" s="20"/>
+      <c r="BC7" s="20"/>
+      <c r="BD7" s="20"/>
+      <c r="BE7" s="20"/>
+      <c r="BF7" s="20"/>
+      <c r="BG7" s="20"/>
+      <c r="BH7" s="20"/>
+      <c r="BI7" s="20"/>
+      <c r="BJ7" s="20"/>
+      <c r="BK7" s="20"/>
+      <c r="BL7" s="20"/>
+      <c r="BM7" s="20"/>
+      <c r="BN7" s="20"/>
+      <c r="BO7" s="20"/>
+      <c r="BP7" s="20"/>
+      <c r="BQ7" s="20"/>
+      <c r="BR7" s="20"/>
+      <c r="BS7" s="20"/>
+      <c r="BT7" s="20"/>
+      <c r="BU7" s="20"/>
+      <c r="BV7" s="20"/>
+    </row>
+    <row r="8" spans="1:74" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
         <v>4</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="19">
         <v>5</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8">
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19">
         <v>1</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="19">
         <v>2</v>
       </c>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8">
+      <c r="O8" s="19"/>
+      <c r="P8" s="19">
         <v>-1</v>
       </c>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8">
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19">
         <v>1</v>
       </c>
-      <c r="U8" s="8">
+      <c r="U8" s="19">
         <v>2</v>
       </c>
-      <c r="V8" s="9"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="9"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="9"/>
-      <c r="AD8" s="9"/>
-      <c r="AE8" s="9"/>
-      <c r="AF8" s="9"/>
-      <c r="AG8" s="9"/>
-      <c r="AH8" s="9"/>
-      <c r="AI8" s="9"/>
-      <c r="AJ8" s="9"/>
-      <c r="AK8" s="9"/>
-      <c r="AL8" s="9"/>
-      <c r="AM8" s="9"/>
-      <c r="AN8" s="9"/>
-      <c r="AO8" s="9"/>
-      <c r="AP8" s="9"/>
-      <c r="AQ8" s="9"/>
-      <c r="AR8" s="9"/>
-      <c r="AS8" s="9"/>
-      <c r="AT8" s="9"/>
-      <c r="AU8" s="9"/>
-      <c r="AV8" s="9"/>
-      <c r="AW8" s="9"/>
-      <c r="AX8" s="9"/>
-      <c r="AY8" s="9"/>
-      <c r="AZ8" s="9"/>
-      <c r="BA8" s="9"/>
-      <c r="BB8" s="9"/>
-      <c r="BC8" s="9"/>
-      <c r="BD8" s="9"/>
-      <c r="BE8" s="9"/>
-      <c r="BF8" s="9"/>
-      <c r="BG8" s="9"/>
-      <c r="BH8" s="9"/>
-      <c r="BI8" s="9"/>
-      <c r="BJ8" s="9"/>
-      <c r="BK8" s="9"/>
-      <c r="BL8" s="9"/>
-      <c r="BM8" s="9"/>
-      <c r="BN8" s="9"/>
-      <c r="BO8" s="9"/>
-      <c r="BP8" s="9"/>
-      <c r="BQ8" s="9"/>
-      <c r="BR8" s="9"/>
-      <c r="BS8" s="9"/>
-      <c r="BT8" s="9"/>
-      <c r="BU8" s="9"/>
-      <c r="BV8" s="9"/>
-    </row>
-    <row r="9" spans="1:74" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>5</v>
-      </c>
-      <c r="B9" s="7" t="s">
+      <c r="V8" s="20"/>
+      <c r="W8" s="19"/>
+      <c r="X8" s="19"/>
+      <c r="Y8" s="19"/>
+      <c r="Z8" s="19"/>
+      <c r="AA8" s="20"/>
+      <c r="AB8" s="20"/>
+      <c r="AC8" s="20"/>
+      <c r="AD8" s="20"/>
+      <c r="AE8" s="20"/>
+      <c r="AF8" s="20"/>
+      <c r="AG8" s="20"/>
+      <c r="AH8" s="20"/>
+      <c r="AI8" s="20"/>
+      <c r="AJ8" s="20"/>
+      <c r="AK8" s="20"/>
+      <c r="AL8" s="20"/>
+      <c r="AM8" s="20"/>
+      <c r="AN8" s="20"/>
+      <c r="AO8" s="20"/>
+      <c r="AP8" s="20"/>
+      <c r="AQ8" s="20"/>
+      <c r="AR8" s="20"/>
+      <c r="AS8" s="20"/>
+      <c r="AT8" s="20"/>
+      <c r="AU8" s="20"/>
+      <c r="AV8" s="20"/>
+      <c r="AW8" s="20"/>
+      <c r="AX8" s="20"/>
+      <c r="AY8" s="20"/>
+      <c r="AZ8" s="20"/>
+      <c r="BA8" s="20"/>
+      <c r="BB8" s="20"/>
+      <c r="BC8" s="20"/>
+      <c r="BD8" s="20"/>
+      <c r="BE8" s="20"/>
+      <c r="BF8" s="20"/>
+      <c r="BG8" s="20"/>
+      <c r="BH8" s="20"/>
+      <c r="BI8" s="20"/>
+      <c r="BJ8" s="20"/>
+      <c r="BK8" s="20"/>
+      <c r="BL8" s="20"/>
+      <c r="BM8" s="20"/>
+      <c r="BN8" s="20"/>
+      <c r="BO8" s="20"/>
+      <c r="BP8" s="20"/>
+      <c r="BQ8" s="20"/>
+      <c r="BR8" s="20"/>
+      <c r="BS8" s="20"/>
+      <c r="BT8" s="20"/>
+      <c r="BU8" s="20"/>
+      <c r="BV8" s="20"/>
+    </row>
+    <row r="9" spans="1:74" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="23"/>
+      <c r="B9" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="16">
-        <v>6</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="9"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="8"/>
-      <c r="AA9" s="9"/>
-      <c r="AB9" s="9"/>
-      <c r="AC9" s="9"/>
-      <c r="AD9" s="9"/>
-      <c r="AE9" s="9"/>
-      <c r="AF9" s="9"/>
-      <c r="AG9" s="9"/>
-      <c r="AH9" s="9"/>
-      <c r="AI9" s="9"/>
-      <c r="AJ9" s="9"/>
-      <c r="AK9" s="9"/>
-      <c r="AL9" s="9"/>
-      <c r="AM9" s="9"/>
-      <c r="AN9" s="9"/>
-      <c r="AO9" s="9"/>
-      <c r="AP9" s="9"/>
-      <c r="AQ9" s="9"/>
-      <c r="AR9" s="9"/>
-      <c r="AS9" s="9"/>
-      <c r="AT9" s="9"/>
-      <c r="AU9" s="9"/>
-      <c r="AV9" s="9"/>
-      <c r="AW9" s="9"/>
-      <c r="AX9" s="9"/>
-      <c r="AY9" s="9"/>
-      <c r="AZ9" s="9"/>
-      <c r="BA9" s="9"/>
-      <c r="BB9" s="9"/>
-      <c r="BC9" s="9"/>
-      <c r="BD9" s="9"/>
-      <c r="BE9" s="9"/>
-      <c r="BF9" s="9"/>
-      <c r="BG9" s="9"/>
-      <c r="BH9" s="9"/>
-      <c r="BI9" s="9"/>
-      <c r="BJ9" s="9"/>
-      <c r="BK9" s="9"/>
-      <c r="BL9" s="9"/>
-      <c r="BM9" s="9"/>
-      <c r="BN9" s="9"/>
-      <c r="BO9" s="9"/>
-      <c r="BP9" s="9"/>
-      <c r="BQ9" s="9"/>
-      <c r="BR9" s="9"/>
-      <c r="BS9" s="9"/>
-      <c r="BT9" s="9"/>
-      <c r="BU9" s="9"/>
-      <c r="BV9" s="9"/>
+      <c r="C9" s="15">
+        <v>4</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="26"/>
+      <c r="W9" s="25"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
+      <c r="AA9" s="26"/>
+      <c r="AB9" s="26"/>
+      <c r="AC9" s="26"/>
+      <c r="AD9" s="26"/>
+      <c r="AE9" s="26"/>
+      <c r="AF9" s="26"/>
+      <c r="AG9" s="26"/>
+      <c r="AH9" s="26"/>
+      <c r="AI9" s="26"/>
+      <c r="AJ9" s="26"/>
+      <c r="AK9" s="26"/>
+      <c r="AL9" s="26"/>
+      <c r="AM9" s="26"/>
+      <c r="AN9" s="26"/>
+      <c r="AO9" s="26"/>
+      <c r="AP9" s="26"/>
+      <c r="AQ9" s="26"/>
+      <c r="AR9" s="26"/>
+      <c r="AS9" s="26"/>
+      <c r="AT9" s="26"/>
+      <c r="AU9" s="26"/>
+      <c r="AV9" s="26"/>
+      <c r="AW9" s="26"/>
+      <c r="AX9" s="26"/>
+      <c r="AY9" s="26"/>
+      <c r="AZ9" s="26"/>
+      <c r="BA9" s="26"/>
+      <c r="BB9" s="26"/>
+      <c r="BC9" s="26"/>
+      <c r="BD9" s="26"/>
+      <c r="BE9" s="26"/>
+      <c r="BF9" s="26"/>
+      <c r="BG9" s="26"/>
+      <c r="BH9" s="26"/>
+      <c r="BI9" s="26"/>
+      <c r="BJ9" s="26"/>
+      <c r="BK9" s="26"/>
+      <c r="BL9" s="26"/>
+      <c r="BM9" s="26"/>
+      <c r="BN9" s="26"/>
+      <c r="BO9" s="26"/>
+      <c r="BP9" s="26"/>
+      <c r="BQ9" s="26"/>
+      <c r="BR9" s="26"/>
+      <c r="BS9" s="26"/>
+      <c r="BT9" s="26"/>
+      <c r="BU9" s="26"/>
+      <c r="BV9" s="26"/>
     </row>
     <row r="10" spans="1:74" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -2946,8 +3086,8 @@
       <c r="B10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="16">
-        <v>7</v>
+      <c r="C10" s="15">
+        <v>5</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -3021,1163 +3161,1287 @@
       <c r="BU10" s="9"/>
       <c r="BV10" s="9"/>
     </row>
-    <row r="11" spans="1:74" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+    <row r="11" spans="1:74" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
         <v>7</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="19">
         <v>3</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
-      <c r="AA11" s="9"/>
-      <c r="AB11" s="9"/>
-      <c r="AC11" s="9"/>
-      <c r="AD11" s="9"/>
-      <c r="AE11" s="9"/>
-      <c r="AF11" s="9"/>
-      <c r="AG11" s="9"/>
-      <c r="AH11" s="9"/>
-      <c r="AI11" s="9"/>
-      <c r="AJ11" s="9"/>
-      <c r="AK11" s="9"/>
-      <c r="AL11" s="9"/>
-      <c r="AM11" s="9"/>
-      <c r="AN11" s="9"/>
-      <c r="AO11" s="9"/>
-      <c r="AP11" s="9"/>
-      <c r="AQ11" s="9"/>
-      <c r="AR11" s="9"/>
-      <c r="AS11" s="9"/>
-      <c r="AT11" s="9"/>
-      <c r="AU11" s="9"/>
-      <c r="AV11" s="9"/>
-      <c r="AW11" s="9"/>
-      <c r="AX11" s="9"/>
-      <c r="AY11" s="9"/>
-      <c r="AZ11" s="9"/>
-      <c r="BA11" s="9"/>
-      <c r="BB11" s="9"/>
-      <c r="BC11" s="9"/>
-      <c r="BD11" s="9"/>
-      <c r="BE11" s="9"/>
-      <c r="BF11" s="9"/>
-      <c r="BG11" s="9"/>
-      <c r="BH11" s="9"/>
-      <c r="BI11" s="9"/>
-      <c r="BJ11" s="9"/>
-      <c r="BK11" s="9"/>
-      <c r="BL11" s="9"/>
-      <c r="BM11" s="9"/>
-      <c r="BN11" s="9"/>
-      <c r="BO11" s="9"/>
-      <c r="BP11" s="9"/>
-      <c r="BQ11" s="9"/>
-      <c r="BR11" s="9"/>
-      <c r="BS11" s="9"/>
-      <c r="BT11" s="9"/>
-      <c r="BU11" s="9"/>
-      <c r="BV11" s="9"/>
-    </row>
-    <row r="12" spans="1:74" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19">
+        <v>1</v>
+      </c>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19">
+        <v>1</v>
+      </c>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="20"/>
+      <c r="AB11" s="20"/>
+      <c r="AC11" s="20">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="20"/>
+      <c r="AE11" s="20"/>
+      <c r="AF11" s="20"/>
+      <c r="AG11" s="20"/>
+      <c r="AH11" s="20"/>
+      <c r="AI11" s="20"/>
+      <c r="AJ11" s="20"/>
+      <c r="AK11" s="20"/>
+      <c r="AL11" s="20"/>
+      <c r="AM11" s="20"/>
+      <c r="AN11" s="20"/>
+      <c r="AO11" s="20"/>
+      <c r="AP11" s="20"/>
+      <c r="AQ11" s="20"/>
+      <c r="AR11" s="20"/>
+      <c r="AS11" s="20"/>
+      <c r="AT11" s="20"/>
+      <c r="AU11" s="20"/>
+      <c r="AV11" s="20"/>
+      <c r="AW11" s="20"/>
+      <c r="AX11" s="20"/>
+      <c r="AY11" s="20"/>
+      <c r="AZ11" s="20"/>
+      <c r="BA11" s="20"/>
+      <c r="BB11" s="20"/>
+      <c r="BC11" s="20"/>
+      <c r="BD11" s="20"/>
+      <c r="BE11" s="20"/>
+      <c r="BF11" s="20"/>
+      <c r="BG11" s="20"/>
+      <c r="BH11" s="20"/>
+      <c r="BI11" s="20"/>
+      <c r="BJ11" s="20"/>
+      <c r="BK11" s="20"/>
+      <c r="BL11" s="20"/>
+      <c r="BM11" s="20"/>
+      <c r="BN11" s="20"/>
+      <c r="BO11" s="20"/>
+      <c r="BP11" s="20"/>
+      <c r="BQ11" s="20"/>
+      <c r="BR11" s="20"/>
+      <c r="BS11" s="20"/>
+      <c r="BT11" s="20"/>
+      <c r="BU11" s="20"/>
+      <c r="BV11" s="20"/>
+    </row>
+    <row r="12" spans="1:74" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
         <v>8</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="19">
         <v>5</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="8"/>
-      <c r="AA12" s="9">
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
+      <c r="X12" s="19"/>
+      <c r="Y12" s="19"/>
+      <c r="Z12" s="19"/>
+      <c r="AA12" s="20">
         <v>1</v>
       </c>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="9">
+      <c r="AB12" s="20"/>
+      <c r="AC12" s="20">
         <v>2</v>
       </c>
-      <c r="AD12" s="9">
+      <c r="AD12" s="20">
         <v>1</v>
       </c>
-      <c r="AE12" s="9">
+      <c r="AE12" s="20">
         <v>1</v>
       </c>
-      <c r="AF12" s="9"/>
-      <c r="AG12" s="9"/>
-      <c r="AH12" s="9"/>
-      <c r="AI12" s="9"/>
-      <c r="AJ12" s="9"/>
-      <c r="AK12" s="9"/>
-      <c r="AL12" s="9"/>
-      <c r="AM12" s="9"/>
-      <c r="AN12" s="9"/>
-      <c r="AO12" s="9"/>
-      <c r="AP12" s="9"/>
-      <c r="AQ12" s="9"/>
-      <c r="AR12" s="9"/>
-      <c r="AS12" s="9"/>
-      <c r="AT12" s="9"/>
-      <c r="AU12" s="9"/>
-      <c r="AV12" s="9"/>
-      <c r="AW12" s="9"/>
-      <c r="AX12" s="9"/>
-      <c r="AY12" s="9"/>
-      <c r="AZ12" s="9"/>
-      <c r="BA12" s="9"/>
-      <c r="BB12" s="9"/>
-      <c r="BC12" s="9"/>
-      <c r="BD12" s="9"/>
-      <c r="BE12" s="9"/>
-      <c r="BF12" s="9"/>
-      <c r="BG12" s="9"/>
-      <c r="BH12" s="9"/>
-      <c r="BI12" s="9"/>
-      <c r="BJ12" s="9"/>
-      <c r="BK12" s="9"/>
-      <c r="BL12" s="9"/>
-      <c r="BM12" s="9"/>
-      <c r="BN12" s="9"/>
-      <c r="BO12" s="9"/>
-      <c r="BP12" s="9"/>
-      <c r="BQ12" s="9"/>
-      <c r="BR12" s="9"/>
-      <c r="BS12" s="9"/>
-      <c r="BT12" s="9"/>
-      <c r="BU12" s="9"/>
-      <c r="BV12" s="9"/>
-    </row>
-    <row r="13" spans="1:74" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="AF12" s="20"/>
+      <c r="AG12" s="20"/>
+      <c r="AH12" s="20"/>
+      <c r="AI12" s="20"/>
+      <c r="AJ12" s="20"/>
+      <c r="AK12" s="20"/>
+      <c r="AL12" s="20"/>
+      <c r="AM12" s="20"/>
+      <c r="AN12" s="20"/>
+      <c r="AO12" s="20"/>
+      <c r="AP12" s="20"/>
+      <c r="AQ12" s="20"/>
+      <c r="AR12" s="20"/>
+      <c r="AS12" s="20"/>
+      <c r="AT12" s="20"/>
+      <c r="AU12" s="20"/>
+      <c r="AV12" s="20"/>
+      <c r="AW12" s="20"/>
+      <c r="AX12" s="20"/>
+      <c r="AY12" s="20"/>
+      <c r="AZ12" s="20"/>
+      <c r="BA12" s="20"/>
+      <c r="BB12" s="20"/>
+      <c r="BC12" s="20"/>
+      <c r="BD12" s="20"/>
+      <c r="BE12" s="20"/>
+      <c r="BF12" s="20"/>
+      <c r="BG12" s="20"/>
+      <c r="BH12" s="20"/>
+      <c r="BI12" s="20"/>
+      <c r="BJ12" s="20"/>
+      <c r="BK12" s="20"/>
+      <c r="BL12" s="20"/>
+      <c r="BM12" s="20"/>
+      <c r="BN12" s="20"/>
+      <c r="BO12" s="20"/>
+      <c r="BP12" s="20"/>
+      <c r="BQ12" s="20"/>
+      <c r="BR12" s="20"/>
+      <c r="BS12" s="20"/>
+      <c r="BT12" s="20"/>
+      <c r="BU12" s="20"/>
+      <c r="BV12" s="20"/>
+    </row>
+    <row r="13" spans="1:74" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
         <v>9</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="19">
         <v>2</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="8"/>
-      <c r="AA13" s="9"/>
-      <c r="AB13" s="9"/>
-      <c r="AC13" s="9"/>
-      <c r="AD13" s="9"/>
-      <c r="AE13" s="9"/>
-      <c r="AF13" s="9"/>
-      <c r="AG13" s="9"/>
-      <c r="AH13" s="9"/>
-      <c r="AI13" s="9"/>
-      <c r="AJ13" s="9">
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
+      <c r="X13" s="19"/>
+      <c r="Y13" s="19"/>
+      <c r="Z13" s="19"/>
+      <c r="AA13" s="20"/>
+      <c r="AB13" s="20"/>
+      <c r="AC13" s="20"/>
+      <c r="AD13" s="20"/>
+      <c r="AE13" s="20"/>
+      <c r="AF13" s="20"/>
+      <c r="AG13" s="20"/>
+      <c r="AH13" s="20"/>
+      <c r="AI13" s="20"/>
+      <c r="AJ13" s="20">
         <v>2</v>
       </c>
-      <c r="AK13" s="9"/>
-      <c r="AL13" s="9"/>
-      <c r="AM13" s="9"/>
-      <c r="AN13" s="9"/>
-      <c r="AO13" s="9"/>
-      <c r="AP13" s="9"/>
-      <c r="AQ13" s="9"/>
-      <c r="AR13" s="9"/>
-      <c r="AS13" s="9"/>
-      <c r="AT13" s="9"/>
-      <c r="AU13" s="9"/>
-      <c r="AV13" s="9"/>
-      <c r="AW13" s="9"/>
-      <c r="AX13" s="9"/>
-      <c r="AY13" s="9"/>
-      <c r="AZ13" s="9"/>
-      <c r="BA13" s="9"/>
-      <c r="BB13" s="9"/>
-      <c r="BC13" s="9"/>
-      <c r="BD13" s="9"/>
-      <c r="BE13" s="9"/>
-      <c r="BF13" s="9"/>
-      <c r="BG13" s="9"/>
-      <c r="BH13" s="9"/>
-      <c r="BI13" s="9"/>
-      <c r="BJ13" s="9"/>
-      <c r="BK13" s="9"/>
-      <c r="BL13" s="9"/>
-      <c r="BM13" s="9"/>
-      <c r="BN13" s="9"/>
-      <c r="BO13" s="9"/>
-      <c r="BP13" s="9"/>
-      <c r="BQ13" s="9"/>
-      <c r="BR13" s="9"/>
-      <c r="BS13" s="9"/>
-      <c r="BT13" s="9"/>
-      <c r="BU13" s="9"/>
-      <c r="BV13" s="9"/>
-    </row>
-    <row r="14" spans="1:74" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="AK13" s="20"/>
+      <c r="AL13" s="20"/>
+      <c r="AM13" s="20"/>
+      <c r="AN13" s="20"/>
+      <c r="AO13" s="20"/>
+      <c r="AP13" s="20"/>
+      <c r="AQ13" s="20"/>
+      <c r="AR13" s="20"/>
+      <c r="AS13" s="20"/>
+      <c r="AT13" s="20"/>
+      <c r="AU13" s="20"/>
+      <c r="AV13" s="20"/>
+      <c r="AW13" s="20"/>
+      <c r="AX13" s="20"/>
+      <c r="AY13" s="20"/>
+      <c r="AZ13" s="20"/>
+      <c r="BA13" s="20"/>
+      <c r="BB13" s="20"/>
+      <c r="BC13" s="20"/>
+      <c r="BD13" s="20"/>
+      <c r="BE13" s="20"/>
+      <c r="BF13" s="20"/>
+      <c r="BG13" s="20"/>
+      <c r="BH13" s="20"/>
+      <c r="BI13" s="20"/>
+      <c r="BJ13" s="20"/>
+      <c r="BK13" s="20"/>
+      <c r="BL13" s="20"/>
+      <c r="BM13" s="20"/>
+      <c r="BN13" s="20"/>
+      <c r="BO13" s="20"/>
+      <c r="BP13" s="20"/>
+      <c r="BQ13" s="20"/>
+      <c r="BR13" s="20"/>
+      <c r="BS13" s="20"/>
+      <c r="BT13" s="20"/>
+      <c r="BU13" s="20"/>
+      <c r="BV13" s="20"/>
+    </row>
+    <row r="14" spans="1:74" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
         <v>10</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="19">
         <v>4</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="8"/>
-      <c r="AA14" s="9"/>
-      <c r="AB14" s="9"/>
-      <c r="AC14" s="9"/>
-      <c r="AD14" s="9"/>
-      <c r="AE14" s="9"/>
-      <c r="AF14" s="9"/>
-      <c r="AG14" s="9"/>
-      <c r="AH14" s="9"/>
-      <c r="AI14" s="9"/>
-      <c r="AJ14" s="9"/>
-      <c r="AK14" s="9"/>
-      <c r="AL14" s="9">
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="20"/>
+      <c r="AB14" s="20"/>
+      <c r="AC14" s="20"/>
+      <c r="AD14" s="20"/>
+      <c r="AE14" s="20"/>
+      <c r="AF14" s="20"/>
+      <c r="AG14" s="20"/>
+      <c r="AH14" s="20"/>
+      <c r="AI14" s="20"/>
+      <c r="AJ14" s="20"/>
+      <c r="AK14" s="20"/>
+      <c r="AL14" s="20">
         <v>1</v>
       </c>
-      <c r="AM14" s="9">
+      <c r="AM14" s="20">
         <v>1</v>
       </c>
-      <c r="AN14" s="9"/>
-      <c r="AO14" s="9">
+      <c r="AN14" s="20"/>
+      <c r="AO14" s="20">
         <v>2</v>
       </c>
-      <c r="AP14" s="9"/>
-      <c r="AQ14" s="9"/>
-      <c r="AR14" s="9"/>
-      <c r="AS14" s="9"/>
-      <c r="AT14" s="9"/>
-      <c r="AU14" s="9"/>
-      <c r="AV14" s="9"/>
-      <c r="AW14" s="9"/>
-      <c r="AX14" s="9"/>
-      <c r="AY14" s="9"/>
-      <c r="AZ14" s="9"/>
-      <c r="BA14" s="9"/>
-      <c r="BB14" s="9"/>
-      <c r="BC14" s="9"/>
-      <c r="BD14" s="9"/>
-      <c r="BE14" s="9"/>
-      <c r="BF14" s="9"/>
-      <c r="BG14" s="9"/>
-      <c r="BH14" s="9"/>
-      <c r="BI14" s="9"/>
-      <c r="BJ14" s="9"/>
-      <c r="BK14" s="9"/>
-      <c r="BL14" s="9"/>
-      <c r="BM14" s="9"/>
-      <c r="BN14" s="9"/>
-      <c r="BO14" s="9"/>
-      <c r="BP14" s="9"/>
-      <c r="BQ14" s="9"/>
-      <c r="BR14" s="9"/>
-      <c r="BS14" s="9"/>
-      <c r="BT14" s="9"/>
-      <c r="BU14" s="9"/>
-      <c r="BV14" s="9"/>
-    </row>
-    <row r="15" spans="1:74" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="AP14" s="20"/>
+      <c r="AQ14" s="20"/>
+      <c r="AR14" s="20"/>
+      <c r="AS14" s="20"/>
+      <c r="AT14" s="20"/>
+      <c r="AU14" s="20"/>
+      <c r="AV14" s="20"/>
+      <c r="AW14" s="20"/>
+      <c r="AX14" s="20"/>
+      <c r="AY14" s="20"/>
+      <c r="AZ14" s="20"/>
+      <c r="BA14" s="20"/>
+      <c r="BB14" s="20"/>
+      <c r="BC14" s="20"/>
+      <c r="BD14" s="20"/>
+      <c r="BE14" s="20"/>
+      <c r="BF14" s="20"/>
+      <c r="BG14" s="20"/>
+      <c r="BH14" s="20"/>
+      <c r="BI14" s="20"/>
+      <c r="BJ14" s="20"/>
+      <c r="BK14" s="20"/>
+      <c r="BL14" s="20"/>
+      <c r="BM14" s="20"/>
+      <c r="BN14" s="20"/>
+      <c r="BO14" s="20"/>
+      <c r="BP14" s="20"/>
+      <c r="BQ14" s="20"/>
+      <c r="BR14" s="20"/>
+      <c r="BS14" s="20"/>
+      <c r="BT14" s="20"/>
+      <c r="BU14" s="20"/>
+      <c r="BV14" s="20"/>
+    </row>
+    <row r="15" spans="1:74" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
         <v>11</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="19">
         <v>3</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="8"/>
-      <c r="AA15" s="9"/>
-      <c r="AB15" s="9"/>
-      <c r="AC15" s="9"/>
-      <c r="AD15" s="9"/>
-      <c r="AE15" s="9"/>
-      <c r="AF15" s="9"/>
-      <c r="AG15" s="9"/>
-      <c r="AH15" s="9"/>
-      <c r="AI15" s="9"/>
-      <c r="AJ15" s="9"/>
-      <c r="AK15" s="9"/>
-      <c r="AL15" s="9"/>
-      <c r="AM15" s="9"/>
-      <c r="AN15" s="9"/>
-      <c r="AO15" s="9"/>
-      <c r="AP15" s="9"/>
-      <c r="AQ15" s="9"/>
-      <c r="AR15" s="9">
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="19"/>
+      <c r="X15" s="19"/>
+      <c r="Y15" s="19"/>
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="20"/>
+      <c r="AB15" s="20"/>
+      <c r="AC15" s="20"/>
+      <c r="AD15" s="20"/>
+      <c r="AE15" s="20"/>
+      <c r="AF15" s="20"/>
+      <c r="AG15" s="20"/>
+      <c r="AH15" s="20"/>
+      <c r="AI15" s="20"/>
+      <c r="AJ15" s="20"/>
+      <c r="AK15" s="20"/>
+      <c r="AL15" s="20"/>
+      <c r="AM15" s="20"/>
+      <c r="AN15" s="20"/>
+      <c r="AO15" s="20"/>
+      <c r="AP15" s="20"/>
+      <c r="AQ15" s="20"/>
+      <c r="AR15" s="20">
         <v>2</v>
       </c>
-      <c r="AS15" s="9">
+      <c r="AS15" s="20">
         <v>1</v>
       </c>
-      <c r="AT15" s="9"/>
-      <c r="AU15" s="9"/>
-      <c r="AV15" s="9"/>
-      <c r="AW15" s="9"/>
-      <c r="AX15" s="9"/>
-      <c r="AY15" s="9"/>
-      <c r="AZ15" s="9"/>
-      <c r="BA15" s="9"/>
-      <c r="BB15" s="9"/>
-      <c r="BC15" s="9"/>
-      <c r="BD15" s="9"/>
-      <c r="BE15" s="9"/>
-      <c r="BF15" s="9"/>
-      <c r="BG15" s="9"/>
-      <c r="BH15" s="9"/>
-      <c r="BI15" s="9"/>
-      <c r="BJ15" s="9"/>
-      <c r="BK15" s="9"/>
-      <c r="BL15" s="9"/>
-      <c r="BM15" s="9"/>
-      <c r="BN15" s="9"/>
-      <c r="BO15" s="9"/>
-      <c r="BP15" s="9"/>
-      <c r="BQ15" s="9"/>
-      <c r="BR15" s="9"/>
-      <c r="BS15" s="9"/>
-      <c r="BT15" s="9"/>
-      <c r="BU15" s="9"/>
-      <c r="BV15" s="9"/>
-    </row>
-    <row r="16" spans="1:74" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="AT15" s="20"/>
+      <c r="AU15" s="20"/>
+      <c r="AV15" s="20"/>
+      <c r="AW15" s="20"/>
+      <c r="AX15" s="20"/>
+      <c r="AY15" s="20"/>
+      <c r="AZ15" s="20"/>
+      <c r="BA15" s="20"/>
+      <c r="BB15" s="20"/>
+      <c r="BC15" s="20"/>
+      <c r="BD15" s="20"/>
+      <c r="BE15" s="20"/>
+      <c r="BF15" s="20"/>
+      <c r="BG15" s="20"/>
+      <c r="BH15" s="20"/>
+      <c r="BI15" s="20"/>
+      <c r="BJ15" s="20"/>
+      <c r="BK15" s="20"/>
+      <c r="BL15" s="20"/>
+      <c r="BM15" s="20"/>
+      <c r="BN15" s="20"/>
+      <c r="BO15" s="20"/>
+      <c r="BP15" s="20"/>
+      <c r="BQ15" s="20"/>
+      <c r="BR15" s="20"/>
+      <c r="BS15" s="20"/>
+      <c r="BT15" s="20"/>
+      <c r="BU15" s="20"/>
+      <c r="BV15" s="20"/>
+    </row>
+    <row r="16" spans="1:74" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="17">
         <v>12</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="19">
         <v>2</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="8"/>
-      <c r="Z16" s="8"/>
-      <c r="AA16" s="9"/>
-      <c r="AB16" s="9"/>
-      <c r="AC16" s="9"/>
-      <c r="AD16" s="9"/>
-      <c r="AE16" s="9"/>
-      <c r="AF16" s="9"/>
-      <c r="AG16" s="9"/>
-      <c r="AH16" s="9"/>
-      <c r="AI16" s="9"/>
-      <c r="AJ16" s="9"/>
-      <c r="AK16" s="9"/>
-      <c r="AL16" s="9"/>
-      <c r="AM16" s="9"/>
-      <c r="AN16" s="9"/>
-      <c r="AO16" s="9"/>
-      <c r="AP16" s="9"/>
-      <c r="AQ16" s="9"/>
-      <c r="AR16" s="9"/>
-      <c r="AS16" s="9"/>
-      <c r="AT16" s="9"/>
-      <c r="AU16" s="9">
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="19"/>
+      <c r="X16" s="19"/>
+      <c r="Y16" s="19"/>
+      <c r="Z16" s="19"/>
+      <c r="AA16" s="20"/>
+      <c r="AB16" s="20"/>
+      <c r="AC16" s="20"/>
+      <c r="AD16" s="20"/>
+      <c r="AE16" s="20"/>
+      <c r="AF16" s="20"/>
+      <c r="AG16" s="20"/>
+      <c r="AH16" s="20"/>
+      <c r="AI16" s="20"/>
+      <c r="AJ16" s="20"/>
+      <c r="AK16" s="20"/>
+      <c r="AL16" s="20"/>
+      <c r="AM16" s="20"/>
+      <c r="AN16" s="20"/>
+      <c r="AO16" s="20"/>
+      <c r="AP16" s="20"/>
+      <c r="AQ16" s="20"/>
+      <c r="AR16" s="20"/>
+      <c r="AS16" s="20"/>
+      <c r="AT16" s="20"/>
+      <c r="AU16" s="20">
         <v>2</v>
       </c>
-      <c r="AV16" s="9"/>
-      <c r="AW16" s="9"/>
-      <c r="AX16" s="9"/>
-      <c r="AY16" s="9"/>
-      <c r="AZ16" s="9"/>
-      <c r="BA16" s="9"/>
-      <c r="BB16" s="9"/>
-      <c r="BC16" s="9"/>
-      <c r="BD16" s="9"/>
-      <c r="BE16" s="9"/>
-      <c r="BF16" s="9"/>
-      <c r="BG16" s="9"/>
-      <c r="BH16" s="9"/>
-      <c r="BI16" s="9"/>
-      <c r="BJ16" s="9"/>
-      <c r="BK16" s="9"/>
-      <c r="BL16" s="9"/>
-      <c r="BM16" s="9"/>
-      <c r="BN16" s="9"/>
-      <c r="BO16" s="9"/>
-      <c r="BP16" s="9"/>
-      <c r="BQ16" s="9"/>
-      <c r="BR16" s="9"/>
-      <c r="BS16" s="9"/>
-      <c r="BT16" s="9"/>
-      <c r="BU16" s="9"/>
-      <c r="BV16" s="9"/>
-    </row>
-    <row r="17" spans="1:74" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="11" t="s">
+      <c r="AV16" s="20"/>
+      <c r="AW16" s="20"/>
+      <c r="AX16" s="20"/>
+      <c r="AY16" s="20"/>
+      <c r="AZ16" s="20"/>
+      <c r="BA16" s="20"/>
+      <c r="BB16" s="20"/>
+      <c r="BC16" s="20"/>
+      <c r="BD16" s="20"/>
+      <c r="BE16" s="20"/>
+      <c r="BF16" s="20"/>
+      <c r="BG16" s="20"/>
+      <c r="BH16" s="20"/>
+      <c r="BI16" s="20"/>
+      <c r="BJ16" s="20"/>
+      <c r="BK16" s="20"/>
+      <c r="BL16" s="20"/>
+      <c r="BM16" s="20"/>
+      <c r="BN16" s="20"/>
+      <c r="BO16" s="20"/>
+      <c r="BP16" s="20"/>
+      <c r="BQ16" s="20"/>
+      <c r="BR16" s="20"/>
+      <c r="BS16" s="20"/>
+      <c r="BT16" s="20"/>
+      <c r="BU16" s="20"/>
+      <c r="BV16" s="20"/>
+    </row>
+    <row r="17" spans="1:74" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17">
+        <v>13</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="19">
+        <v>4</v>
+      </c>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19"/>
+      <c r="X17" s="19"/>
+      <c r="Y17" s="19"/>
+      <c r="Z17" s="19"/>
+      <c r="AA17" s="20"/>
+      <c r="AB17" s="20"/>
+      <c r="AC17" s="20"/>
+      <c r="AD17" s="20"/>
+      <c r="AE17" s="20"/>
+      <c r="AF17" s="20"/>
+      <c r="AG17" s="20"/>
+      <c r="AH17" s="20"/>
+      <c r="AI17" s="20"/>
+      <c r="AJ17" s="20"/>
+      <c r="AK17" s="20"/>
+      <c r="AL17" s="20"/>
+      <c r="AM17" s="20"/>
+      <c r="AN17" s="20"/>
+      <c r="AO17" s="20"/>
+      <c r="AP17" s="20"/>
+      <c r="AQ17" s="20"/>
+      <c r="AR17" s="20"/>
+      <c r="AS17" s="20"/>
+      <c r="AT17" s="20"/>
+      <c r="AU17" s="20"/>
+      <c r="AV17" s="20"/>
+      <c r="AW17" s="20"/>
+      <c r="AX17" s="20"/>
+      <c r="AY17" s="20"/>
+      <c r="AZ17" s="20"/>
+      <c r="BA17" s="20"/>
+      <c r="BB17" s="20"/>
+      <c r="BC17" s="20"/>
+      <c r="BD17" s="20"/>
+      <c r="BE17" s="20"/>
+      <c r="BF17" s="20"/>
+      <c r="BG17" s="20"/>
+      <c r="BH17" s="20"/>
+      <c r="BI17" s="20"/>
+      <c r="BJ17" s="20"/>
+      <c r="BK17" s="20"/>
+      <c r="BL17" s="20">
+        <v>2</v>
+      </c>
+      <c r="BM17" s="20">
+        <v>1</v>
+      </c>
+      <c r="BN17" s="20">
+        <v>1</v>
+      </c>
+      <c r="BO17" s="20"/>
+      <c r="BP17" s="20"/>
+      <c r="BQ17" s="20"/>
+      <c r="BR17" s="20"/>
+      <c r="BS17" s="20"/>
+      <c r="BT17" s="20"/>
+      <c r="BU17" s="20"/>
+      <c r="BV17" s="20"/>
+    </row>
+    <row r="18" spans="1:74" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
+        <v>14</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="19">
+        <v>4</v>
+      </c>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="19"/>
+      <c r="W18" s="19"/>
+      <c r="X18" s="19"/>
+      <c r="Y18" s="19"/>
+      <c r="Z18" s="19"/>
+      <c r="AA18" s="20"/>
+      <c r="AB18" s="20"/>
+      <c r="AC18" s="20"/>
+      <c r="AD18" s="20"/>
+      <c r="AE18" s="20"/>
+      <c r="AF18" s="20"/>
+      <c r="AG18" s="20"/>
+      <c r="AH18" s="20"/>
+      <c r="AI18" s="20"/>
+      <c r="AJ18" s="20"/>
+      <c r="AK18" s="20"/>
+      <c r="AL18" s="20"/>
+      <c r="AM18" s="20"/>
+      <c r="AN18" s="20"/>
+      <c r="AO18" s="20"/>
+      <c r="AP18" s="20"/>
+      <c r="AQ18" s="20"/>
+      <c r="AR18" s="20"/>
+      <c r="AS18" s="20"/>
+      <c r="AT18" s="20"/>
+      <c r="AU18" s="20"/>
+      <c r="AV18" s="20"/>
+      <c r="AW18" s="20"/>
+      <c r="AX18" s="20"/>
+      <c r="AY18" s="20"/>
+      <c r="AZ18" s="20"/>
+      <c r="BA18" s="20"/>
+      <c r="BB18" s="20"/>
+      <c r="BC18" s="20"/>
+      <c r="BD18" s="20"/>
+      <c r="BE18" s="20"/>
+      <c r="BF18" s="20">
+        <v>3</v>
+      </c>
+      <c r="BG18" s="20"/>
+      <c r="BH18" s="20"/>
+      <c r="BI18" s="20">
+        <v>1</v>
+      </c>
+      <c r="BJ18" s="20"/>
+      <c r="BK18" s="20"/>
+      <c r="BL18" s="20"/>
+      <c r="BM18" s="20"/>
+      <c r="BN18" s="20"/>
+      <c r="BO18" s="20"/>
+      <c r="BP18" s="20"/>
+      <c r="BQ18" s="20"/>
+      <c r="BR18" s="20"/>
+      <c r="BS18" s="20"/>
+      <c r="BT18" s="20"/>
+      <c r="BU18" s="20"/>
+      <c r="BV18" s="20"/>
+    </row>
+    <row r="19" spans="1:74" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="12">
-        <f>SUM(C5:C16)</f>
+      <c r="C19" s="11">
+        <f>SUM(C5:C18)</f>
+        <v>50</v>
+      </c>
+      <c r="D19" s="11">
+        <f>C19-SUM(D5:D18)</f>
+        <v>50</v>
+      </c>
+      <c r="E19" s="11">
+        <f t="shared" ref="E19:BP19" si="0">D19-SUM(E5:E18)</f>
+        <v>49</v>
+      </c>
+      <c r="F19" s="11">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="G19" s="11">
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="D17" s="12">
-        <f>C17-SUM(D5:D16)</f>
-        <v>46</v>
-      </c>
-      <c r="E17" s="12">
-        <f>D17-SUM(E5:E16)</f>
+      <c r="H19" s="11">
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="F17" s="12">
-        <f>E17-SUM(F5:F16)</f>
-        <v>43</v>
-      </c>
-      <c r="G17" s="12">
-        <f>F17-SUM(G5:G16)</f>
-        <v>42</v>
-      </c>
-      <c r="H17" s="12">
-        <f>G17-SUM(H5:H16)</f>
+      <c r="I19" s="11">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="J19" s="11">
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="I17" s="12">
-        <f>H17-SUM(I5:I16)</f>
+      <c r="K19" s="11">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="L19" s="11">
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="J17" s="12">
-        <f>I17-SUM(J5:J16)</f>
+      <c r="M19" s="11">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="N19" s="11">
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="K17" s="12">
-        <f>J17-SUM(K5:K16)</f>
+      <c r="O19" s="11">
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="L17" s="12">
-        <f>K17-SUM(L5:L16)</f>
+      <c r="P19" s="11">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="Q19" s="11">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="R19" s="11">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="S19" s="11">
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="M17" s="12">
-        <f>L17-SUM(M5:M16)</f>
+      <c r="T19" s="11">
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="N17" s="12">
-        <f>M17-SUM(N5:N16)</f>
+      <c r="U19" s="11">
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="O17" s="12">
-        <f>N17-SUM(O5:O16)</f>
+      <c r="V19" s="11">
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="P17" s="12">
-        <f>O17-SUM(P5:P16)</f>
-        <v>35</v>
-      </c>
-      <c r="Q17" s="12">
-        <f>P17-SUM(Q5:Q16)</f>
-        <v>35</v>
-      </c>
-      <c r="R17" s="12">
-        <f>Q17-SUM(R5:R16)</f>
-        <v>35</v>
-      </c>
-      <c r="S17" s="12">
-        <f>R17-SUM(S5:S16)</f>
-        <v>35</v>
-      </c>
-      <c r="T17" s="12">
-        <f>S17-SUM(T5:T16)</f>
+      <c r="W19" s="11">
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="U17" s="12">
-        <f>T17-SUM(U5:U16)</f>
-        <v>32</v>
-      </c>
-      <c r="V17" s="12">
-        <f>U17-SUM(V5:V16)</f>
-        <v>32</v>
-      </c>
-      <c r="W17" s="12">
-        <f>V17-SUM(W5:W16)</f>
-        <v>32</v>
-      </c>
-      <c r="X17" s="12">
-        <f>W17-SUM(X5:X16)</f>
-        <v>32</v>
-      </c>
-      <c r="Y17" s="12">
-        <f>X17-SUM(Y5:Y16)</f>
-        <v>32</v>
-      </c>
-      <c r="Z17" s="12">
-        <f>Y17-SUM(Z5:Z16)</f>
-        <v>32</v>
-      </c>
-      <c r="AA17" s="12">
-        <f>Z17-SUM(AA5:AA16)</f>
-        <v>31</v>
-      </c>
-      <c r="AB17" s="12">
-        <f>AA17-SUM(AB5:AB16)</f>
-        <v>31</v>
-      </c>
-      <c r="AC17" s="12">
-        <f>AB17-SUM(AC5:AC16)</f>
+      <c r="X19" s="11">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="Y19" s="11">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="Z19" s="11">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="AA19" s="11">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="AB19" s="11">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="AC19" s="11">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="AD19" s="11">
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="AD17" s="12">
-        <f>AC17-SUM(AD5:AD16)</f>
+      <c r="AE19" s="11">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="AE17" s="12">
-        <f>AD17-SUM(AE5:AE16)</f>
-        <v>27</v>
-      </c>
-      <c r="AF17" s="12">
-        <f>AE17-SUM(AF5:AF16)</f>
-        <v>27</v>
-      </c>
-      <c r="AG17" s="12">
-        <f>AF17-SUM(AG5:AG16)</f>
-        <v>27</v>
-      </c>
-      <c r="AH17" s="12">
-        <f>AG17-SUM(AH5:AH16)</f>
-        <v>27</v>
-      </c>
-      <c r="AI17" s="12">
-        <f>AH17-SUM(AI5:AI16)</f>
-        <v>27</v>
-      </c>
-      <c r="AJ17" s="12">
-        <f>AI17-SUM(AJ5:AJ16)</f>
+      <c r="AF19" s="11">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="AG19" s="11">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="AH19" s="11">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="AI19" s="11">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="AJ19" s="11">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="AK19" s="11">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="AL19" s="11">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="AK17" s="12">
-        <f>AJ17-SUM(AK5:AK16)</f>
-        <v>25</v>
-      </c>
-      <c r="AL17" s="12">
-        <f>AK17-SUM(AL5:AL16)</f>
+      <c r="AM19" s="11">
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AM17" s="12">
-        <f>AL17-SUM(AM5:AM16)</f>
-        <v>23</v>
-      </c>
-      <c r="AN17" s="12">
-        <f>AM17-SUM(AN5:AN16)</f>
-        <v>23</v>
-      </c>
-      <c r="AO17" s="12">
-        <f>AN17-SUM(AO5:AO16)</f>
-        <v>21</v>
-      </c>
-      <c r="AP17" s="12">
-        <f>AO17-SUM(AP5:AP16)</f>
-        <v>21</v>
-      </c>
-      <c r="AQ17" s="12">
-        <f>AP17-SUM(AQ5:AQ16)</f>
-        <v>21</v>
-      </c>
-      <c r="AR17" s="12">
-        <f>AQ17-SUM(AR5:AR16)</f>
+      <c r="AN19" s="11">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="AO19" s="11">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="AP19" s="11">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="AQ19" s="11">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="AR19" s="11">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="AS19" s="11">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="AS17" s="12">
-        <f>AR17-SUM(AS5:AS16)</f>
-        <v>18</v>
-      </c>
-      <c r="AT17" s="12">
-        <f>AS17-SUM(AT5:AT16)</f>
-        <v>18</v>
-      </c>
-      <c r="AU17" s="12">
-        <f>AT17-SUM(AU5:AU16)</f>
-        <v>16</v>
-      </c>
-      <c r="AV17" s="12">
-        <f>AU17-SUM(AV5:AV16)</f>
-        <v>16</v>
-      </c>
-      <c r="AW17" s="12">
-        <f>AV17-SUM(AW5:AW16)</f>
-        <v>16</v>
-      </c>
-      <c r="AX17" s="12">
-        <f>AW17-SUM(AX5:AX16)</f>
-        <v>16</v>
-      </c>
-      <c r="AY17" s="12">
-        <f>AX17-SUM(AY5:AY16)</f>
-        <v>16</v>
-      </c>
-      <c r="AZ17" s="12">
-        <f>AY17-SUM(AZ5:AZ16)</f>
-        <v>16</v>
-      </c>
-      <c r="BA17" s="12">
-        <f>AZ17-SUM(BA5:BA16)</f>
-        <v>16</v>
-      </c>
-      <c r="BB17" s="12">
-        <f>BA17-SUM(BB5:BB16)</f>
-        <v>16</v>
-      </c>
-      <c r="BC17" s="12">
-        <f>BB17-SUM(BC5:BC16)</f>
-        <v>16</v>
-      </c>
-      <c r="BD17" s="12">
-        <f>BC17-SUM(BD5:BD16)</f>
-        <v>16</v>
-      </c>
-      <c r="BE17" s="12">
-        <f>BD17-SUM(BE5:BE16)</f>
-        <v>16</v>
-      </c>
-      <c r="BF17" s="12">
-        <f>BE17-SUM(BF5:BF16)</f>
-        <v>16</v>
-      </c>
-      <c r="BG17" s="12">
-        <f>BF17-SUM(BG5:BG16)</f>
-        <v>16</v>
-      </c>
-      <c r="BH17" s="12">
-        <f>BG17-SUM(BH5:BH16)</f>
-        <v>16</v>
-      </c>
-      <c r="BI17" s="12">
-        <f>BH17-SUM(BI5:BI16)</f>
-        <v>16</v>
-      </c>
-      <c r="BJ17" s="12">
-        <f>BI17-SUM(BJ5:BJ16)</f>
-        <v>16</v>
-      </c>
-      <c r="BK17" s="12">
-        <f>BJ17-SUM(BK5:BK16)</f>
-        <v>16</v>
-      </c>
-      <c r="BL17" s="12">
-        <f>BK17-SUM(BL5:BL16)</f>
-        <v>16</v>
-      </c>
-      <c r="BM17" s="12">
-        <f>BL17-SUM(BM5:BM16)</f>
-        <v>16</v>
-      </c>
-      <c r="BN17" s="12">
-        <f>BM17-SUM(BN5:BN16)</f>
-        <v>16</v>
-      </c>
-      <c r="BO17" s="12">
-        <f>BN17-SUM(BO5:BO16)</f>
-        <v>16</v>
-      </c>
-      <c r="BP17" s="12">
-        <f>BO17-SUM(BP5:BP16)</f>
-        <v>16</v>
-      </c>
-      <c r="BQ17" s="12">
-        <f>BP17-SUM(BQ5:BQ16)</f>
-        <v>16</v>
-      </c>
-      <c r="BR17" s="12">
-        <f>BQ17-SUM(BR5:BR16)</f>
-        <v>16</v>
-      </c>
-      <c r="BS17" s="12">
-        <f>BR17-SUM(BS5:BS16)</f>
-        <v>16</v>
-      </c>
-      <c r="BT17" s="12">
-        <f>BS17-SUM(BT5:BT16)</f>
-        <v>16</v>
-      </c>
-      <c r="BU17" s="12">
-        <f>BT17-SUM(BU5:BU16)</f>
-        <v>16</v>
-      </c>
-      <c r="BV17" s="12">
-        <f>BU17-SUM(BV5:BV16)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:74" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="13" t="s">
+      <c r="AT19" s="11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="AU19" s="11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="AV19" s="11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="AW19" s="11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="AX19" s="11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="AY19" s="11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="AZ19" s="11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="BA19" s="11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="BB19" s="11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="BC19" s="11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="BD19" s="11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="BE19" s="11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="BF19" s="11">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="BG19" s="11">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="BH19" s="11">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="BI19" s="11">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="BJ19" s="11">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="BK19" s="11">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="BL19" s="11">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="BM19" s="11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="BN19" s="11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="BO19" s="11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="BP19" s="11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="BQ19" s="11">
+        <f t="shared" ref="BQ19:BV19" si="1">BP19-SUM(BQ5:BQ18)</f>
+        <v>9</v>
+      </c>
+      <c r="BR19" s="11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="BS19" s="11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="BT19" s="11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="BU19" s="11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="BV19" s="11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:74" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="14">
-        <f>SUM(C5:C16)</f>
-        <v>46</v>
-      </c>
-      <c r="D18" s="15">
-        <f>$C$18-($C$18/71*1)</f>
-        <v>45.352112676056336</v>
-      </c>
-      <c r="E18" s="15">
-        <f>$C$18-($C$18/71*2)</f>
-        <v>44.704225352112672</v>
-      </c>
-      <c r="F18" s="15">
-        <f>$C$18-($C$18/71*3)</f>
-        <v>44.056338028169016</v>
-      </c>
-      <c r="G18" s="15">
-        <f>$C$18-($C$18/71*4)</f>
-        <v>43.408450704225352</v>
-      </c>
-      <c r="H18" s="15">
-        <f>$C$18-($C$18/71*5)</f>
-        <v>42.760563380281688</v>
-      </c>
-      <c r="I18" s="15">
-        <f>$C$18-($C$18/71*6)</f>
-        <v>42.112676056338032</v>
-      </c>
-      <c r="J18" s="15">
-        <f>$C$18-($C$18/71*7)</f>
-        <v>41.464788732394368</v>
-      </c>
-      <c r="K18" s="15">
-        <f>$C$18-($C$18/71*8)</f>
-        <v>40.816901408450704</v>
-      </c>
-      <c r="L18" s="15">
-        <f>$C$18-($C$18/71*9)</f>
-        <v>40.16901408450704</v>
-      </c>
-      <c r="M18" s="15">
-        <f>$C$18-($C$18/71*10)</f>
-        <v>39.521126760563376</v>
-      </c>
-      <c r="N18" s="15">
-        <f>$C$18-($C$18/71*11)</f>
-        <v>38.87323943661972</v>
-      </c>
-      <c r="O18" s="15">
-        <f>$C$18-($C$18/71*12)</f>
-        <v>38.225352112676056</v>
-      </c>
-      <c r="P18" s="15">
-        <f>$C$18-($C$18/71*13)</f>
-        <v>37.577464788732392</v>
-      </c>
-      <c r="Q18" s="15">
-        <f>$C$18-($C$18/71*14)</f>
-        <v>36.929577464788736</v>
-      </c>
-      <c r="R18" s="15">
-        <f>$C$18-($C$18/71*15)</f>
-        <v>36.281690140845072</v>
-      </c>
-      <c r="S18" s="15">
-        <f>$C$18-($C$18/71*16)</f>
-        <v>35.633802816901408</v>
-      </c>
-      <c r="T18" s="15">
-        <f>$C$18-($C$18/71*17)</f>
-        <v>34.985915492957744</v>
-      </c>
-      <c r="U18" s="15">
-        <f>$C$18-($C$18/71*18)</f>
-        <v>34.338028169014081</v>
-      </c>
-      <c r="V18" s="15">
-        <f>$C$18-($C$18/71*19)</f>
-        <v>33.690140845070424</v>
-      </c>
-      <c r="W18" s="15">
-        <f>$C$18-($C$18/71*20)</f>
-        <v>33.04225352112676</v>
-      </c>
-      <c r="X18" s="15">
-        <f>$C$18-($C$18/71*21)</f>
-        <v>32.394366197183096</v>
-      </c>
-      <c r="Y18" s="15">
-        <f>$C$18-($C$18/71*22)</f>
-        <v>31.746478873239436</v>
-      </c>
-      <c r="Z18" s="15">
-        <f>$C$18-($C$18/71*23)</f>
-        <v>31.098591549295776</v>
-      </c>
-      <c r="AA18" s="15">
-        <f>$C$18-($C$18/71*24)</f>
-        <v>30.450704225352112</v>
-      </c>
-      <c r="AB18" s="15">
-        <f>$C$18-($C$18/71*25)</f>
-        <v>29.802816901408448</v>
-      </c>
-      <c r="AC18" s="15">
-        <f>$C$18-($C$18/71*26)</f>
-        <v>29.154929577464788</v>
-      </c>
-      <c r="AD18" s="15">
-        <f>$C$18-($C$18/71*27)</f>
-        <v>28.507042253521128</v>
-      </c>
-      <c r="AE18" s="15">
-        <f>$C$18-($C$18/71*28)</f>
-        <v>27.859154929577464</v>
-      </c>
-      <c r="AF18" s="15">
-        <f>$C$18-($C$18/71*29)</f>
-        <v>27.2112676056338</v>
-      </c>
-      <c r="AG18" s="15">
-        <f>$C$18-($C$18/71*30)</f>
-        <v>26.56338028169014</v>
-      </c>
-      <c r="AH18" s="15">
-        <f>$C$18-($C$18/71*31)</f>
-        <v>25.91549295774648</v>
-      </c>
-      <c r="AI18" s="15">
-        <f>$C$18-($C$18/71*32)</f>
-        <v>25.267605633802816</v>
-      </c>
-      <c r="AJ18" s="15">
-        <f>$C$18-($C$18/71*33)</f>
-        <v>24.619718309859152</v>
-      </c>
-      <c r="AK18" s="15">
-        <f>$C$18-($C$18/71*34)</f>
-        <v>23.971830985915492</v>
-      </c>
-      <c r="AL18" s="15">
-        <f>$C$18-($C$18/71*35)</f>
-        <v>23.323943661971832</v>
-      </c>
-      <c r="AM18" s="15">
-        <f>$C$18-($C$18/71*36)</f>
-        <v>22.676056338028168</v>
-      </c>
-      <c r="AN18" s="15">
-        <f>$C$18-($C$18/71*37)</f>
-        <v>22.028169014084504</v>
-      </c>
-      <c r="AO18" s="15">
-        <f>$C$18-($C$18/71*38)</f>
-        <v>21.380281690140844</v>
-      </c>
-      <c r="AP18" s="15">
-        <f>$C$18-($C$18/71*39)</f>
-        <v>20.732394366197184</v>
-      </c>
-      <c r="AQ18" s="15">
-        <f>$C$18-($C$18/71*40)</f>
-        <v>20.08450704225352</v>
-      </c>
-      <c r="AR18" s="15">
-        <f>$C$18-($C$18/71*41)</f>
-        <v>19.436619718309856</v>
-      </c>
-      <c r="AS18" s="15">
-        <f>$C$18-($C$18/71*42)</f>
-        <v>18.788732394366196</v>
-      </c>
-      <c r="AT18" s="15">
-        <f>$C$18-($C$18/71*43)</f>
-        <v>18.140845070422536</v>
-      </c>
-      <c r="AU18" s="15">
-        <f>$C$18-($C$18/71*44)</f>
-        <v>17.492957746478872</v>
-      </c>
-      <c r="AV18" s="15">
-        <f>$C$18-($C$18/71*45)</f>
-        <v>16.845070422535208</v>
-      </c>
-      <c r="AW18" s="15">
-        <f>$C$18-($C$18/71*46)</f>
-        <v>16.197183098591548</v>
-      </c>
-      <c r="AX18" s="15">
-        <f>$C$18-($C$18/71*47)</f>
-        <v>15.549295774647888</v>
-      </c>
-      <c r="AY18" s="15">
-        <f>$C$18-($C$18/71*48)</f>
-        <v>14.901408450704224</v>
-      </c>
-      <c r="AZ18" s="15">
-        <f>$C$18-($C$18/71*49)</f>
-        <v>14.25352112676056</v>
-      </c>
-      <c r="BA18" s="15">
-        <f>$C$18-($C$18/71*50)</f>
-        <v>13.605633802816897</v>
-      </c>
-      <c r="BB18" s="15">
-        <f>$C$18-($C$18/71*51)</f>
-        <v>12.95774647887324</v>
-      </c>
-      <c r="BC18" s="15">
-        <f>$C$18-($C$18/71*52)</f>
-        <v>12.309859154929576</v>
-      </c>
-      <c r="BD18" s="15">
-        <f>$C$18-($C$18/71*53)</f>
-        <v>11.661971830985912</v>
-      </c>
-      <c r="BE18" s="15">
-        <f>$C$18-($C$18/71*54)</f>
-        <v>11.014084507042256</v>
-      </c>
-      <c r="BF18" s="15">
-        <f>$C$18-($C$18/71*55)</f>
-        <v>10.366197183098592</v>
-      </c>
-      <c r="BG18" s="15">
-        <f>$C$18-($C$18/71*56)</f>
-        <v>9.7183098591549282</v>
-      </c>
-      <c r="BH18" s="15">
-        <f>$C$18-($C$18/71*57)</f>
-        <v>9.0704225352112644</v>
-      </c>
-      <c r="BI18" s="15">
-        <f>$C$18-($C$18/71*58)</f>
-        <v>8.4225352112676006</v>
-      </c>
-      <c r="BJ18" s="15">
-        <f>$C$18-($C$18/71*59)</f>
-        <v>7.774647887323944</v>
-      </c>
-      <c r="BK18" s="15">
-        <f>$C$18-($C$18/71*60)</f>
-        <v>7.1267605633802802</v>
-      </c>
-      <c r="BL18" s="15">
-        <f>$C$18-($C$18/71*61)</f>
-        <v>6.4788732394366164</v>
-      </c>
-      <c r="BM18" s="15">
-        <f>$C$18-($C$18/71*62)</f>
-        <v>5.8309859154929597</v>
-      </c>
-      <c r="BN18" s="15">
-        <f>$C$18-($C$18/71*63)</f>
-        <v>5.183098591549296</v>
-      </c>
-      <c r="BO18" s="15">
-        <f>$C$18-($C$18/71*64)</f>
-        <v>4.5352112676056322</v>
-      </c>
-      <c r="BP18" s="15">
-        <f>$C$18-($C$18/71*65)</f>
-        <v>3.8873239436619684</v>
-      </c>
-      <c r="BQ18" s="15">
-        <f>$C$18-($C$18/71*66)</f>
-        <v>3.2394366197183047</v>
-      </c>
-      <c r="BR18" s="15">
-        <f>$C$18-($C$18/71*67)</f>
-        <v>2.591549295774648</v>
-      </c>
-      <c r="BS18" s="15">
-        <f>$C$18-($C$18/71*68)</f>
-        <v>1.9436619718309842</v>
-      </c>
-      <c r="BT18" s="15">
-        <f>$C$18-($C$18/71*69)</f>
-        <v>1.2957746478873204</v>
-      </c>
-      <c r="BU18" s="15">
-        <f>$C$18-($C$18/71*70)</f>
-        <v>0.64788732394366377</v>
-      </c>
-      <c r="BV18" s="15">
-        <f>$C$18-($C$18/71*71)</f>
+      <c r="C20" s="13">
+        <f>SUM(C5:C18)</f>
+        <v>50</v>
+      </c>
+      <c r="D20" s="14">
+        <f>$C$20-($C$20/71*1)</f>
+        <v>49.295774647887328</v>
+      </c>
+      <c r="E20" s="14">
+        <f>$C$20-($C$20/71*2)</f>
+        <v>48.591549295774648</v>
+      </c>
+      <c r="F20" s="14">
+        <f>$C$20-($C$20/71*3)</f>
+        <v>47.887323943661968</v>
+      </c>
+      <c r="G20" s="14">
+        <f>$C$20-($C$20/71*4)</f>
+        <v>47.183098591549296</v>
+      </c>
+      <c r="H20" s="14">
+        <f>$C$20-($C$20/71*5)</f>
+        <v>46.478873239436624</v>
+      </c>
+      <c r="I20" s="14">
+        <f>$C$20-($C$20/71*6)</f>
+        <v>45.774647887323944</v>
+      </c>
+      <c r="J20" s="14">
+        <f>$C$20-($C$20/71*7)</f>
+        <v>45.070422535211264</v>
+      </c>
+      <c r="K20" s="14">
+        <f>$C$20-($C$20/71*8)</f>
+        <v>44.366197183098592</v>
+      </c>
+      <c r="L20" s="14">
+        <f>$C$20-($C$20/71*9)</f>
+        <v>43.661971830985919</v>
+      </c>
+      <c r="M20" s="14">
+        <f>$C$20-($C$20/71*10)</f>
+        <v>42.95774647887324</v>
+      </c>
+      <c r="N20" s="14">
+        <f>$C$20-($C$20/71*11)</f>
+        <v>42.25352112676056</v>
+      </c>
+      <c r="O20" s="14">
+        <f>$C$20-($C$20/71*12)</f>
+        <v>41.549295774647888</v>
+      </c>
+      <c r="P20" s="14">
+        <f>$C$20-($C$20/71*13)</f>
+        <v>40.845070422535215</v>
+      </c>
+      <c r="Q20" s="14">
+        <f>$C$20-($C$20/71*14)</f>
+        <v>40.140845070422536</v>
+      </c>
+      <c r="R20" s="14">
+        <f>$C$20-($C$20/71*15)</f>
+        <v>39.436619718309856</v>
+      </c>
+      <c r="S20" s="14">
+        <f>$C$20-($C$20/71*16)</f>
+        <v>38.732394366197184</v>
+      </c>
+      <c r="T20" s="14">
+        <f>$C$20-($C$20/71*17)</f>
+        <v>38.028169014084511</v>
+      </c>
+      <c r="U20" s="14">
+        <f>$C$20-($C$20/71*18)</f>
+        <v>37.323943661971832</v>
+      </c>
+      <c r="V20" s="14">
+        <f>$C$20-($C$20/71*19)</f>
+        <v>36.619718309859152</v>
+      </c>
+      <c r="W20" s="14">
+        <f>$C$20-($C$20/71*20)</f>
+        <v>35.91549295774648</v>
+      </c>
+      <c r="X20" s="14">
+        <f>$C$20-($C$20/71*21)</f>
+        <v>35.211267605633807</v>
+      </c>
+      <c r="Y20" s="14">
+        <f>$C$20-($C$20/71*22)</f>
+        <v>34.507042253521128</v>
+      </c>
+      <c r="Z20" s="14">
+        <f>$C$20-($C$20/71*23)</f>
+        <v>33.802816901408448</v>
+      </c>
+      <c r="AA20" s="14">
+        <f>$C$20-($C$20/71*24)</f>
+        <v>33.098591549295776</v>
+      </c>
+      <c r="AB20" s="14">
+        <f>$C$20-($C$20/71*25)</f>
+        <v>32.394366197183103</v>
+      </c>
+      <c r="AC20" s="14">
+        <f>$C$20-($C$20/71*26)</f>
+        <v>31.690140845070424</v>
+      </c>
+      <c r="AD20" s="14">
+        <f>$C$20-($C$20/71*27)</f>
+        <v>30.985915492957748</v>
+      </c>
+      <c r="AE20" s="14">
+        <f>$C$20-($C$20/71*28)</f>
+        <v>30.281690140845072</v>
+      </c>
+      <c r="AF20" s="14">
+        <f>$C$20-($C$20/71*29)</f>
+        <v>29.577464788732396</v>
+      </c>
+      <c r="AG20" s="14">
+        <f>$C$20-($C$20/71*30)</f>
+        <v>28.87323943661972</v>
+      </c>
+      <c r="AH20" s="14">
+        <f>$C$20-($C$20/71*31)</f>
+        <v>28.169014084507044</v>
+      </c>
+      <c r="AI20" s="14">
+        <f>$C$20-($C$20/71*32)</f>
+        <v>27.464788732394368</v>
+      </c>
+      <c r="AJ20" s="14">
+        <f>$C$20-($C$20/71*33)</f>
+        <v>26.760563380281692</v>
+      </c>
+      <c r="AK20" s="14">
+        <f>$C$20-($C$20/71*34)</f>
+        <v>26.056338028169016</v>
+      </c>
+      <c r="AL20" s="14">
+        <f>$C$20-($C$20/71*35)</f>
+        <v>25.35211267605634</v>
+      </c>
+      <c r="AM20" s="14">
+        <f>$C$20-($C$20/71*36)</f>
+        <v>24.647887323943664</v>
+      </c>
+      <c r="AN20" s="14">
+        <f>$C$20-($C$20/71*37)</f>
+        <v>23.943661971830988</v>
+      </c>
+      <c r="AO20" s="14">
+        <f>$C$20-($C$20/71*38)</f>
+        <v>23.239436619718312</v>
+      </c>
+      <c r="AP20" s="14">
+        <f>$C$20-($C$20/71*39)</f>
+        <v>22.535211267605636</v>
+      </c>
+      <c r="AQ20" s="14">
+        <f>$C$20-($C$20/71*40)</f>
+        <v>21.83098591549296</v>
+      </c>
+      <c r="AR20" s="14">
+        <f>$C$20-($C$20/71*41)</f>
+        <v>21.126760563380284</v>
+      </c>
+      <c r="AS20" s="14">
+        <f>$C$20-($C$20/71*42)</f>
+        <v>20.422535211267608</v>
+      </c>
+      <c r="AT20" s="14">
+        <f>$C$20-($C$20/71*43)</f>
+        <v>19.718309859154932</v>
+      </c>
+      <c r="AU20" s="14">
+        <f>$C$20-($C$20/71*44)</f>
+        <v>19.014084507042256</v>
+      </c>
+      <c r="AV20" s="14">
+        <f>$C$20-($C$20/71*45)</f>
+        <v>18.30985915492958</v>
+      </c>
+      <c r="AW20" s="14">
+        <f>$C$20-($C$20/71*46)</f>
+        <v>17.605633802816904</v>
+      </c>
+      <c r="AX20" s="14">
+        <f>$C$20-($C$20/71*47)</f>
+        <v>16.901408450704224</v>
+      </c>
+      <c r="AY20" s="14">
+        <f>$C$20-($C$20/71*48)</f>
+        <v>16.197183098591552</v>
+      </c>
+      <c r="AZ20" s="14">
+        <f>$C$20-($C$20/71*49)</f>
+        <v>15.492957746478879</v>
+      </c>
+      <c r="BA20" s="14">
+        <f>$C$20-($C$20/71*50)</f>
+        <v>14.7887323943662</v>
+      </c>
+      <c r="BB20" s="14">
+        <f>$C$20-($C$20/71*51)</f>
+        <v>14.08450704225352</v>
+      </c>
+      <c r="BC20" s="14">
+        <f>$C$20-($C$20/71*52)</f>
+        <v>13.380281690140848</v>
+      </c>
+      <c r="BD20" s="14">
+        <f>$C$20-($C$20/71*53)</f>
+        <v>12.676056338028175</v>
+      </c>
+      <c r="BE20" s="14">
+        <f>$C$20-($C$20/71*54)</f>
+        <v>11.971830985915496</v>
+      </c>
+      <c r="BF20" s="14">
+        <f>$C$20-($C$20/71*55)</f>
+        <v>11.267605633802816</v>
+      </c>
+      <c r="BG20" s="14">
+        <f>$C$20-($C$20/71*56)</f>
+        <v>10.563380281690144</v>
+      </c>
+      <c r="BH20" s="14">
+        <f>$C$20-($C$20/71*57)</f>
+        <v>9.8591549295774712</v>
+      </c>
+      <c r="BI20" s="14">
+        <f>$C$20-($C$20/71*58)</f>
+        <v>9.1549295774647916</v>
+      </c>
+      <c r="BJ20" s="14">
+        <f>$C$20-($C$20/71*59)</f>
+        <v>8.4507042253521121</v>
+      </c>
+      <c r="BK20" s="14">
+        <f>$C$20-($C$20/71*60)</f>
+        <v>7.7464788732394396</v>
+      </c>
+      <c r="BL20" s="14">
+        <f>$C$20-($C$20/71*61)</f>
+        <v>7.0422535211267672</v>
+      </c>
+      <c r="BM20" s="14">
+        <f>$C$20-($C$20/71*62)</f>
+        <v>6.3380281690140876</v>
+      </c>
+      <c r="BN20" s="14">
+        <f>$C$20-($C$20/71*63)</f>
+        <v>5.6338028169014081</v>
+      </c>
+      <c r="BO20" s="14">
+        <f>$C$20-($C$20/71*64)</f>
+        <v>4.9295774647887356</v>
+      </c>
+      <c r="BP20" s="14">
+        <f>$C$20-($C$20/71*65)</f>
+        <v>4.2253521126760631</v>
+      </c>
+      <c r="BQ20" s="14">
+        <f>$C$20-($C$20/71*66)</f>
+        <v>3.5211267605633836</v>
+      </c>
+      <c r="BR20" s="14">
+        <f>$C$20-($C$20/71*67)</f>
+        <v>2.816901408450704</v>
+      </c>
+      <c r="BS20" s="14">
+        <f>$C$20-($C$20/71*68)</f>
+        <v>2.1126760563380316</v>
+      </c>
+      <c r="BT20" s="14">
+        <f>$C$20-($C$20/71*69)</f>
+        <v>1.4084507042253591</v>
+      </c>
+      <c r="BU20" s="14">
+        <f>$C$20-($C$20/71*70)</f>
+        <v>0.70422535211267956</v>
+      </c>
+      <c r="BV20" s="14">
+        <f>$C$20-($C$20/71*71)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
-      <c r="X19" s="2"/>
-      <c r="Y19" s="2"/>
-      <c r="Z19" s="2"/>
-    </row>
-    <row r="20" spans="1:74" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-      <c r="X20" s="2"/>
-      <c r="Y20" s="2"/>
-      <c r="Z20" s="2"/>
     </row>
     <row r="21" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
@@ -31674,6 +31938,62 @@
       <c r="X1002" s="2"/>
       <c r="Y1002" s="2"/>
       <c r="Z1002" s="2"/>
+    </row>
+    <row r="1003" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1003" s="2"/>
+      <c r="B1003" s="2"/>
+      <c r="C1003" s="2"/>
+      <c r="D1003" s="2"/>
+      <c r="E1003" s="2"/>
+      <c r="F1003" s="2"/>
+      <c r="G1003" s="2"/>
+      <c r="H1003" s="2"/>
+      <c r="I1003" s="2"/>
+      <c r="J1003" s="2"/>
+      <c r="K1003" s="2"/>
+      <c r="L1003" s="2"/>
+      <c r="M1003" s="2"/>
+      <c r="N1003" s="2"/>
+      <c r="O1003" s="2"/>
+      <c r="P1003" s="2"/>
+      <c r="Q1003" s="2"/>
+      <c r="R1003" s="2"/>
+      <c r="S1003" s="2"/>
+      <c r="T1003" s="2"/>
+      <c r="U1003" s="2"/>
+      <c r="V1003" s="2"/>
+      <c r="W1003" s="2"/>
+      <c r="X1003" s="2"/>
+      <c r="Y1003" s="2"/>
+      <c r="Z1003" s="2"/>
+    </row>
+    <row r="1004" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1004" s="2"/>
+      <c r="B1004" s="2"/>
+      <c r="C1004" s="2"/>
+      <c r="D1004" s="2"/>
+      <c r="E1004" s="2"/>
+      <c r="F1004" s="2"/>
+      <c r="G1004" s="2"/>
+      <c r="H1004" s="2"/>
+      <c r="I1004" s="2"/>
+      <c r="J1004" s="2"/>
+      <c r="K1004" s="2"/>
+      <c r="L1004" s="2"/>
+      <c r="M1004" s="2"/>
+      <c r="N1004" s="2"/>
+      <c r="O1004" s="2"/>
+      <c r="P1004" s="2"/>
+      <c r="Q1004" s="2"/>
+      <c r="R1004" s="2"/>
+      <c r="S1004" s="2"/>
+      <c r="T1004" s="2"/>
+      <c r="U1004" s="2"/>
+      <c r="V1004" s="2"/>
+      <c r="W1004" s="2"/>
+      <c r="X1004" s="2"/>
+      <c r="Y1004" s="2"/>
+      <c r="Z1004" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -31707,7 +32027,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{647DEFFF-6FDC-48A5-86DD-C67FC497BA52}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC15E989-0340-4167-86DE-6E03F9581888}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>